<commit_message>
update on new studies
</commit_message>
<xml_diff>
--- a/Literature_search/2016-2017.xlsx
+++ b/Literature_search/2016-2017.xlsx
@@ -24,8 +24,116 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="B3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+7th grade</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D3" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+also had some anxiety, etc. questionnaires that are not relevant here
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+8th grade</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D4" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+also had some anxiety, etc. questionnaires that are not relevant here
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="77">
   <si>
     <t>ID</t>
   </si>
@@ -1077,6 +1185,210 @@
   </si>
   <si>
     <r>
+      <t>Grossman, I., &amp; Rajan, R. (2017). The effect of simultaneous text on the recall of noise-degraded speech. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of Experimental Psychology: Human Perception and Performance</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>43</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(5), 986.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Kou, S., McClelland, A., &amp; Furnham, A. (2017). The effect of background music and noise on the cognitive test performance of Chinese introverts and extraverts. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Psychology of Music</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 0305735617704300.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Liu, T., Lin, C. C., Huang, K. C., &amp; Chen, Y. C. (2017). Effects of noise type, noise intensity, and illumination intensity on reading performance. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Applied Acoustics</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>120</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, 70-74.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Sukowski, H., &amp; Romanus, E. (2016, September). Effects of background speech on reading performance in adults. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceedings of Meetings on Acoustics 22ICA</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (Vol. 28, No. 1, p. 050002). ASA.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Wendt, D., Dau, T., &amp; Hjortkjær, J. (2016). Impact of background noise and sentence complexity on processing demands during sentence comprehension. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Frontiers in psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Yan, G., Meng, Z., Liu, N., He, L., &amp; Paterson, K. B. (2017). Effects of Irrelevant Background Speech on Eye Movements during Reading. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The Quarterly Journal of Experimental Psychology</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, (just-accepted), 1-20.</t>
+    </r>
+  </si>
+  <si>
+    <t>Included?</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Reason for exclusion</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>Although students were tested on more than one occasion, the exposure to music occurred only during the actual testing. Therefore, this is not an intervention study; it still meets inclusion criteria</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>2 (background sound: silence vs classical music) x grade (7th, 8th)</t>
+  </si>
+  <si>
+    <r>
       <t>Falcon, E. (2017). </t>
     </r>
     <r>
@@ -1094,210 +1406,64 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t> (Doctoral dissertation, St. Thomas University).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Grossman, I., &amp; Rajan, R. (2017). The effect of simultaneous text on the recall of noise-degraded speech. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Journal of Experimental Psychology: Human Perception and Performance</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>43</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(5), 986.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Kou, S., McClelland, A., &amp; Furnham, A. (2017). The effect of background music and noise on the cognitive test performance of Chinese introverts and extraverts. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Psychology of Music</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, 0305735617704300.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Liu, T., Lin, C. C., Huang, K. C., &amp; Chen, Y. C. (2017). Effects of noise type, noise intensity, and illumination intensity on reading performance. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Applied Acoustics</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>120</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, 70-74.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Sukowski, H., &amp; Romanus, E. (2016, September). Effects of background speech on reading performance in adults. In </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Proceedings of Meetings on Acoustics 22ICA</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t> (Vol. 28, No. 1, p. 050002). ASA.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Wendt, D., Dau, T., &amp; Hjortkjær, J. (2016). Impact of background noise and sentence complexity on processing demands during sentence comprehension. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Frontiers in psychology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Yan, G., Meng, Z., Liu, N., He, L., &amp; Paterson, K. B. (2017). Effects of Irrelevant Background Speech on Eye Movements during Reading. </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>The Quarterly Journal of Experimental Psychology</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>, (just-accepted), 1-20.</t>
-    </r>
-  </si>
-  <si>
-    <t>Included?</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
-    <t>Reason for exclusion</t>
-  </si>
-  <si>
-    <t>Comments</t>
+      <t xml:space="preserve"> (Doctoral dissertation, St. Thomas University)., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample 1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Falcon, E. (2017). </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>The relationship between background classical music and reading comprehension on seventh and eighth grade students</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (Doctoral dissertation, St. Thomas University)., </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Sample 2</t>
+    </r>
+  </si>
+  <si>
+    <t>3 (background sound: silence, liked music, disliked music)</t>
+  </si>
+  <si>
+    <t>Time taken to complete task does not constitute reading speed per se because it also includes the time taken to answer the questions; not coded</t>
+  </si>
+  <si>
+    <t>3 (background sound: silence, office noise, pop music)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1350,6 +1516,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1383,7 +1581,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1423,12 +1621,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2860,24 +3063,25 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="3"/>
-    <col min="2" max="2" width="87" style="6" customWidth="1"/>
+    <col min="2" max="2" width="72.85546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="3" customWidth="1"/>
     <col min="4" max="4" width="20.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.140625" style="3" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" style="3" customWidth="1"/>
     <col min="7" max="7" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
@@ -2889,91 +3093,117 @@
         <v>2</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+    </row>
+    <row r="3" spans="1:7" s="16" customFormat="1" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
         <v>1</v>
       </c>
-      <c r="B3" s="17" t="s">
-        <v>20</v>
+      <c r="B3" s="20" t="s">
+        <v>72</v>
       </c>
       <c r="C3" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15" t="s">
+      <c r="D3" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="16" customFormat="1" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="15">
+    <row r="4" spans="1:7" s="16" customFormat="1" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
         <v>2</v>
       </c>
-      <c r="B4" s="18" t="s">
-        <v>57</v>
+      <c r="B4" s="20" t="s">
+        <v>73</v>
       </c>
       <c r="C4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" s="16" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" s="16" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
         <v>4</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" s="16" customFormat="1" ht="39" x14ac:dyDescent="0.25">
-      <c r="A5" s="15">
-        <v>3</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" s="16" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A6" s="15">
-        <v>4</v>
-      </c>
-      <c r="B6" s="18" t="s">
-        <v>59</v>
+      <c r="B6" s="20" t="s">
+        <v>60</v>
       </c>
       <c r="C6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="15"/>
+      <c r="D6" s="19" t="s">
+        <v>76</v>
+      </c>
       <c r="E6" s="15"/>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="16" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="16" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B7" s="18" t="s">
-        <v>60</v>
+      <c r="B7" s="20" t="s">
+        <v>57</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2981,15 +3211,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="16" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="16" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <v>6</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>61</v>
+        <v>3</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2997,12 +3227,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="16" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="15">
-        <v>7</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>62</v>
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="15"/>
+      <c r="B9" s="17" t="s">
+        <v>58</v>
       </c>
       <c r="C9" s="15" t="s">
         <v>22</v>
@@ -3012,19 +3240,14 @@
       <c r="F9" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="15">
+    </row>
+    <row r="10" spans="1:7" s="16" customFormat="1" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15"/>
+      <c r="B10" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>8</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="15" t="s">
-        <v>4</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3032,31 +3255,30 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="16" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A11" s="15">
-        <v>9</v>
-      </c>
-      <c r="B11" s="18" t="s">
-        <v>63</v>
+    <row r="11" spans="1:7" s="16" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+      <c r="B11" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" s="16" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="15">
-        <v>10</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>64</v>
+      <c r="G11" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="16" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+      <c r="A12" s="15"/>
+      <c r="B12" s="17" t="s">
+        <v>62</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -3064,15 +3286,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="16" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
-        <v>11</v>
-      </c>
-      <c r="B13" s="18" t="s">
-        <v>65</v>
+    <row r="13" spans="1:7" s="16" customFormat="1" ht="42" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+      <c r="B13" s="17" t="s">
+        <v>63</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -3080,7 +3300,27 @@
         <v>38</v>
       </c>
     </row>
+    <row r="14" spans="1:7" s="16" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15"/>
+      <c r="B14" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState ref="A3:G14">
+    <sortCondition ref="A3:A14"/>
+    <sortCondition ref="B3:B14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>